<commit_message>
Shop Page Dev Completed
</commit_message>
<xml_diff>
--- a/Data/Data_set.xlsx
+++ b/Data/Data_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/53a66839347cb57d/Desktop/pythonProject/udemy_course_project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_F25DC773A252ABDACC104894A1DE40A65BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B21B1FF-571E-4B05-ABFC-F53190CDEC1C}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_F25DC773A252ABDACC104894A1DE40A65BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47B9DDC8-BAE4-4A17-9465-ABC17B20E62A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Date Of Birth</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Blackberry</t>
   </si>
 </sst>
 </file>
@@ -119,6 +125,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,11 +394,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -444,6 +452,14 @@
         <v>34406</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{B7937BF8-2BD9-4701-9E0B-0A79D55E3276}"/>

</xml_diff>